<commit_message>
Mise en place de l'algo pour placer les tuiles de couloirs (tuyaux).
</commit_message>
<xml_diff>
--- a/tileset/DungeonGenerator/Escaliers verticaux.xlsx
+++ b/tileset/DungeonGenerator/Escaliers verticaux.xlsx
@@ -55,12 +55,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -164,7 +170,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -180,6 +186,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="90"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M64"/>
+  <dimension ref="B1:S64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -495,9 +502,10 @@
     <col min="12" max="12" width="3.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="3.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="105" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:19" ht="105" x14ac:dyDescent="0.25">
       <c r="J1" s="12" t="s">
         <v>6</v>
       </c>
@@ -505,14 +513,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F3" s="2"/>
       <c r="G3" s="5"/>
       <c r="H3" s="1"/>
@@ -523,7 +531,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F4" s="2"/>
       <c r="G4" s="7"/>
       <c r="H4" s="5"/>
@@ -534,12 +542,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F5" s="8"/>
       <c r="G5" s="2"/>
       <c r="H5" s="4"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F6" s="2"/>
       <c r="G6" s="7"/>
       <c r="H6" s="4"/>
@@ -551,17 +559,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F7" s="8"/>
       <c r="G7" s="2"/>
       <c r="H7" s="4"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F8" s="2"/>
       <c r="G8" s="7"/>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -574,7 +582,7 @@
       <c r="G9" s="2"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C10" s="10" t="s">
         <v>0</v>
       </c>
@@ -584,13 +592,13 @@
       <c r="G10" s="6"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F12" s="2"/>
       <c r="G12" s="5"/>
       <c r="H12" s="1"/>
@@ -600,8 +608,13 @@
       <c r="L12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="Q12" s="13"/>
+      <c r="R12" s="13"/>
+      <c r="S12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F13" s="8"/>
       <c r="G13" s="2"/>
       <c r="H13" s="4"/>
@@ -611,13 +624,14 @@
       <c r="M13" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="Q13" s="13"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F14" s="2"/>
       <c r="G14" s="7"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F15" s="8"/>
       <c r="G15" s="2"/>
       <c r="H15" s="4"/>
@@ -628,13 +642,19 @@
         <f>MOD(J15,2)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="Q15" s="13"/>
+      <c r="R15" s="13"/>
+      <c r="S15">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F16" s="2"/>
       <c r="G16" s="7"/>
       <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="R16" s="13"/>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>1</v>
       </c>
@@ -647,7 +667,7 @@
       <c r="G17" s="2"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C18" s="10" t="s">
         <v>0</v>
       </c>
@@ -656,14 +676,22 @@
       <c r="F18" s="1"/>
       <c r="G18" s="6"/>
       <c r="H18" s="4"/>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="R18" s="13"/>
+      <c r="S18">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C21" s="10" t="s">
         <v>0</v>
       </c>
@@ -671,8 +699,12 @@
       <c r="E21" s="1"/>
       <c r="F21" s="9"/>
       <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="Q21" s="13"/>
+      <c r="S21">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>1</v>
       </c>
@@ -681,8 +713,10 @@
       </c>
       <c r="F22" s="8"/>
       <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F23" s="2"/>
       <c r="G23" s="7"/>
       <c r="J23">
@@ -693,11 +727,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F24" s="8"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F25" s="2"/>
       <c r="G25" s="7"/>
       <c r="H25" s="1"/>
@@ -711,7 +745,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F26" s="8"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
@@ -722,13 +756,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C30" s="10" t="s">
         <v>0</v>
       </c>
@@ -738,7 +772,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="3"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>1</v>
       </c>
@@ -748,7 +782,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
       <c r="F32" s="8"/>
       <c r="G32" s="2"/>
       <c r="J32">

</xml_diff>